<commit_message>
Generating full F20 outputs, including validation after fixing #324 and other issues in previous commits (including error in CM, new version v.6.2.1)
</commit_message>
<xml_diff>
--- a/mappings/package_F20/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F20/transformation/conceptual_mappings.xlsx
@@ -363,7 +363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="779">
   <si>
     <t>Field</t>
   </si>
@@ -398,7 +398,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.2.0</t>
+    <t>6.2.1</t>
   </si>
   <si>
     <r>
@@ -4028,7 +4028,7 @@
     <t>Directive 2014/24/EU – In the case of framework agreements, provide justification for any duration exceeding 4 years</t>
   </si>
   <si>
-    <t>PROCEDURE/CRITERIA_EVALUATION</t>
+    <t>MODIFICATIONS_CONTRACT/DESCRIPTION_PROCUREMENT/JUSTIFICATION</t>
   </si>
   <si>
     <t>epo:Lot / epo:FrameworkAgreementTerm / rdf:langString</t>
@@ -4044,9 +4044,6 @@
   </si>
   <si>
     <t>Directive 2014/25/EU – In the case of framework agreements, provide justification for any duration exceeding 8 years:</t>
-  </si>
-  <si>
-    <t>MODIFICATIONS_CONTRACT/DESCRIPTION_PROCUREMENT/JUSTIFICATION</t>
   </si>
   <si>
     <t>VII.1.6</t>
@@ -13283,7 +13280,7 @@
       <c r="D134" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="E134" s="119" t="s">
+      <c r="E134" s="115" t="s">
         <v>559</v>
       </c>
       <c r="F134" s="49"/>
@@ -13312,8 +13309,8 @@
       <c r="D135" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="E135" s="115" t="s">
-        <v>565</v>
+      <c r="E135" s="119" t="s">
+        <v>559</v>
       </c>
       <c r="F135" s="49"/>
       <c r="G135" s="39" t="s">
@@ -13330,17 +13327,17 @@
     </row>
     <row r="136">
       <c r="A136" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="B136" s="47" t="s">
         <v>566</v>
-      </c>
-      <c r="B136" s="47" t="s">
-        <v>567</v>
       </c>
       <c r="C136" s="110" t="s">
         <v>316</v>
       </c>
       <c r="D136" s="110"/>
       <c r="E136" s="115" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F136" s="115"/>
       <c r="G136" s="36" t="s">
@@ -13355,7 +13352,7 @@
     </row>
     <row r="137">
       <c r="A137" s="63" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B137" s="55" t="s">
         <v>349</v>
@@ -13369,31 +13366,31 @@
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
       <c r="K137" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="63" t="s">
+        <v>570</v>
+      </c>
+      <c r="B138" s="55" t="s">
         <v>571</v>
       </c>
-      <c r="B138" s="55" t="s">
+      <c r="C138" s="120" t="s">
         <v>572</v>
       </c>
-      <c r="C138" s="120" t="s">
+      <c r="D138" s="120" t="s">
         <v>573</v>
       </c>
-      <c r="D138" s="120" t="s">
+      <c r="E138" s="121" t="s">
         <v>574</v>
-      </c>
-      <c r="E138" s="121" t="s">
-        <v>575</v>
       </c>
       <c r="F138" s="39"/>
       <c r="G138" s="4" t="s">
         <v>406</v>
       </c>
       <c r="H138" s="39" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
@@ -13401,7 +13398,7 @@
     </row>
     <row r="139">
       <c r="A139" s="63" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B139" s="55" t="s">
         <v>409</v>
@@ -13411,14 +13408,14 @@
       </c>
       <c r="D139" s="122"/>
       <c r="E139" s="121" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F139" s="39"/>
       <c r="G139" s="4" t="s">
         <v>412</v>
       </c>
       <c r="H139" s="39" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -13426,17 +13423,17 @@
     </row>
     <row r="140">
       <c r="A140" s="63" t="s">
+        <v>579</v>
+      </c>
+      <c r="B140" s="55" t="s">
         <v>580</v>
-      </c>
-      <c r="B140" s="55" t="s">
-        <v>581</v>
       </c>
       <c r="C140" s="120" t="s">
         <v>410</v>
       </c>
       <c r="D140" s="122"/>
       <c r="E140" s="121" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F140" s="39"/>
       <c r="G140" s="4" t="s">
@@ -13448,15 +13445,15 @@
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
       <c r="K140" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="48" t="s">
+        <v>583</v>
+      </c>
+      <c r="B141" s="47" t="s">
         <v>584</v>
-      </c>
-      <c r="B141" s="47" t="s">
-        <v>585</v>
       </c>
       <c r="C141" s="113" t="s">
         <v>316</v>
@@ -13469,12 +13466,12 @@
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
       <c r="K141" s="75" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="63" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B142" s="55" t="s">
         <v>349</v>
@@ -13488,12 +13485,12 @@
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
       <c r="K142" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B143" s="55" t="s">
         <v>57</v>
@@ -13505,14 +13502,14 @@
         <v>59</v>
       </c>
       <c r="E143" s="121" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F143" s="121"/>
       <c r="G143" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H143" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I143" s="7" t="s">
         <v>63</v>
@@ -13522,7 +13519,7 @@
     </row>
     <row r="144">
       <c r="A144" s="63" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B144" s="55" t="s">
         <v>65</v>
@@ -13534,14 +13531,14 @@
         <v>67</v>
       </c>
       <c r="E144" s="121" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F144" s="121"/>
       <c r="G144" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H144" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I144" s="7" t="s">
         <v>71</v>
@@ -13551,7 +13548,7 @@
     </row>
     <row r="145">
       <c r="A145" s="63" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B145" s="55" t="s">
         <v>73</v>
@@ -13563,14 +13560,14 @@
         <v>75</v>
       </c>
       <c r="E145" s="121" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F145" s="121"/>
       <c r="G145" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H145" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
@@ -13578,7 +13575,7 @@
     </row>
     <row r="146">
       <c r="A146" s="63" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B146" s="55" t="s">
         <v>80</v>
@@ -13590,14 +13587,14 @@
         <v>82</v>
       </c>
       <c r="E146" s="121" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F146" s="121"/>
       <c r="G146" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H146" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
@@ -13605,7 +13602,7 @@
     </row>
     <row r="147">
       <c r="A147" s="63" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B147" s="55" t="s">
         <v>86</v>
@@ -13617,26 +13614,26 @@
         <v>88</v>
       </c>
       <c r="E147" s="121" t="s">
+        <v>600</v>
+      </c>
+      <c r="F147" s="121" t="s">
         <v>601</v>
-      </c>
-      <c r="F147" s="121" t="s">
-        <v>602</v>
       </c>
       <c r="G147" s="4" t="s">
         <v>91</v>
       </c>
       <c r="H147" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
       <c r="K147" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="63" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B148" s="55" t="s">
         <v>94</v>
@@ -13648,14 +13645,14 @@
         <v>368</v>
       </c>
       <c r="E148" s="121" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F148" s="121"/>
       <c r="G148" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H148" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
@@ -13663,7 +13660,7 @@
     </row>
     <row r="149">
       <c r="A149" s="63" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B149" s="55" t="s">
         <v>101</v>
@@ -13675,14 +13672,14 @@
         <v>103</v>
       </c>
       <c r="E149" s="121" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F149" s="121"/>
       <c r="G149" s="4" t="s">
         <v>105</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
@@ -13690,7 +13687,7 @@
     </row>
     <row r="150">
       <c r="A150" s="63" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B150" s="55" t="s">
         <v>121</v>
@@ -13702,7 +13699,7 @@
         <v>110</v>
       </c>
       <c r="E150" s="121" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F150" s="121"/>
       <c r="G150" s="4" t="s">
@@ -13717,7 +13714,7 @@
     </row>
     <row r="151">
       <c r="A151" s="63" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B151" s="55" t="s">
         <v>115</v>
@@ -13729,7 +13726,7 @@
         <v>117</v>
       </c>
       <c r="E151" s="121" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F151" s="121"/>
       <c r="G151" s="4" t="s">
@@ -13744,10 +13741,10 @@
     </row>
     <row r="152">
       <c r="A152" s="63" t="s">
+        <v>614</v>
+      </c>
+      <c r="B152" s="55" t="s">
         <v>615</v>
-      </c>
-      <c r="B152" s="55" t="s">
-        <v>616</v>
       </c>
       <c r="C152" s="120" t="s">
         <v>122</v>
@@ -13756,14 +13753,14 @@
         <v>123</v>
       </c>
       <c r="E152" s="121" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F152" s="121"/>
       <c r="G152" s="4" t="s">
         <v>376</v>
       </c>
       <c r="H152" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
@@ -13771,7 +13768,7 @@
     </row>
     <row r="153">
       <c r="A153" s="63" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B153" s="55" t="s">
         <v>128</v>
@@ -13783,7 +13780,7 @@
         <v>130</v>
       </c>
       <c r="E153" s="121" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F153" s="121"/>
       <c r="G153" s="4" t="s">
@@ -13798,34 +13795,34 @@
     </row>
     <row r="154">
       <c r="A154" s="63" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B154" s="55" t="s">
         <v>390</v>
       </c>
       <c r="C154" s="120" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D154" s="122"/>
       <c r="E154" s="121" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F154" s="39"/>
       <c r="G154" s="4" t="s">
         <v>394</v>
       </c>
       <c r="H154" s="95" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
       <c r="K154" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="77" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B155" s="78" t="s">
         <v>390</v>
@@ -13833,14 +13830,14 @@
       <c r="C155" s="120"/>
       <c r="D155" s="122"/>
       <c r="E155" s="119" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F155" s="39"/>
       <c r="G155" s="43" t="s">
         <v>394</v>
       </c>
       <c r="H155" s="124" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
@@ -13848,10 +13845,10 @@
     </row>
     <row r="156">
       <c r="A156" s="83" t="s">
+        <v>625</v>
+      </c>
+      <c r="B156" s="38" t="s">
         <v>626</v>
-      </c>
-      <c r="B156" s="38" t="s">
-        <v>627</v>
       </c>
       <c r="C156" s="110" t="s">
         <v>316</v>
@@ -13867,24 +13864,24 @@
     </row>
     <row r="157">
       <c r="A157" s="48" t="s">
+        <v>627</v>
+      </c>
+      <c r="B157" s="47" t="s">
         <v>628</v>
-      </c>
-      <c r="B157" s="47" t="s">
-        <v>629</v>
       </c>
       <c r="C157" s="120" t="s">
         <v>316</v>
       </c>
       <c r="D157" s="122"/>
       <c r="E157" s="121" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F157" s="121"/>
       <c r="G157" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="H157" s="117" t="s">
         <v>631</v>
-      </c>
-      <c r="H157" s="117" t="s">
-        <v>632</v>
       </c>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
@@ -13892,26 +13889,26 @@
     </row>
     <row r="158">
       <c r="A158" s="63" t="s">
+        <v>632</v>
+      </c>
+      <c r="B158" s="55" t="s">
         <v>633</v>
       </c>
-      <c r="B158" s="55" t="s">
+      <c r="C158" s="120" t="s">
         <v>634</v>
       </c>
-      <c r="C158" s="120" t="s">
+      <c r="D158" s="120" t="s">
         <v>635</v>
       </c>
-      <c r="D158" s="120" t="s">
+      <c r="E158" s="121" t="s">
         <v>636</v>
-      </c>
-      <c r="E158" s="121" t="s">
-        <v>637</v>
       </c>
       <c r="F158" s="121"/>
       <c r="G158" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="H158" s="4" t="s">
         <v>638</v>
-      </c>
-      <c r="H158" s="4" t="s">
-        <v>639</v>
       </c>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
@@ -13919,10 +13916,10 @@
     </row>
     <row r="159">
       <c r="A159" s="48" t="s">
+        <v>639</v>
+      </c>
+      <c r="B159" s="47" t="s">
         <v>640</v>
-      </c>
-      <c r="B159" s="47" t="s">
-        <v>641</v>
       </c>
       <c r="C159" s="120" t="s">
         <v>316</v>
@@ -13938,26 +13935,26 @@
     </row>
     <row r="160">
       <c r="A160" s="63" t="s">
+        <v>641</v>
+      </c>
+      <c r="B160" s="55" t="s">
         <v>642</v>
       </c>
-      <c r="B160" s="55" t="s">
+      <c r="C160" s="120" t="s">
         <v>643</v>
       </c>
-      <c r="C160" s="120" t="s">
+      <c r="D160" s="120" t="s">
         <v>644</v>
       </c>
-      <c r="D160" s="120" t="s">
+      <c r="E160" s="121" t="s">
         <v>645</v>
-      </c>
-      <c r="E160" s="121" t="s">
-        <v>646</v>
       </c>
       <c r="F160" s="121"/>
       <c r="G160" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="H160" s="125" t="s">
         <v>647</v>
-      </c>
-      <c r="H160" s="125" t="s">
-        <v>648</v>
       </c>
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
@@ -13965,26 +13962,26 @@
     </row>
     <row r="161">
       <c r="A161" s="63" t="s">
+        <v>648</v>
+      </c>
+      <c r="B161" s="73" t="s">
         <v>649</v>
       </c>
-      <c r="B161" s="73" t="s">
+      <c r="C161" s="120" t="s">
         <v>650</v>
       </c>
-      <c r="C161" s="120" t="s">
+      <c r="D161" s="120" t="s">
         <v>651</v>
       </c>
-      <c r="D161" s="120" t="s">
-        <v>652</v>
-      </c>
       <c r="E161" s="118" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F161" s="126"/>
       <c r="G161" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H161" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
@@ -13992,26 +13989,26 @@
     </row>
     <row r="162">
       <c r="A162" s="63" t="s">
+        <v>653</v>
+      </c>
+      <c r="B162" s="73" t="s">
         <v>654</v>
       </c>
-      <c r="B162" s="73" t="s">
+      <c r="C162" s="120" t="s">
+        <v>643</v>
+      </c>
+      <c r="D162" s="120" t="s">
+        <v>644</v>
+      </c>
+      <c r="E162" s="126" t="s">
         <v>655</v>
-      </c>
-      <c r="C162" s="120" t="s">
-        <v>644</v>
-      </c>
-      <c r="D162" s="120" t="s">
-        <v>645</v>
-      </c>
-      <c r="E162" s="126" t="s">
-        <v>656</v>
       </c>
       <c r="F162" s="126"/>
       <c r="G162" s="7" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H162" s="127" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I162" s="7"/>
       <c r="J162" s="7"/>
@@ -14019,26 +14016,26 @@
     </row>
     <row r="163">
       <c r="A163" s="63" t="s">
+        <v>657</v>
+      </c>
+      <c r="B163" s="73" t="s">
         <v>658</v>
       </c>
-      <c r="B163" s="73" t="s">
-        <v>659</v>
-      </c>
       <c r="C163" s="120" t="s">
+        <v>650</v>
+      </c>
+      <c r="D163" s="120" t="s">
         <v>651</v>
       </c>
-      <c r="D163" s="120" t="s">
-        <v>652</v>
-      </c>
       <c r="E163" s="118" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F163" s="126"/>
       <c r="G163" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H163" s="128" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I163" s="7"/>
       <c r="J163" s="7"/>
@@ -14046,10 +14043,10 @@
     </row>
     <row r="164">
       <c r="A164" s="48" t="s">
+        <v>659</v>
+      </c>
+      <c r="B164" s="62" t="s">
         <v>660</v>
-      </c>
-      <c r="B164" s="62" t="s">
-        <v>661</v>
       </c>
       <c r="C164" s="120" t="s">
         <v>316</v>
@@ -14065,7 +14062,7 @@
     </row>
     <row r="165">
       <c r="A165" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B165" s="73" t="s">
         <v>349</v>
@@ -14079,29 +14076,29 @@
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
       <c r="K165" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="63" t="s">
+        <v>662</v>
+      </c>
+      <c r="B166" s="73" t="s">
         <v>663</v>
       </c>
-      <c r="B166" s="73" t="s">
-        <v>664</v>
-      </c>
       <c r="C166" s="129" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D166" s="130"/>
       <c r="E166" s="131" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F166" s="131"/>
       <c r="G166" s="132" t="s">
         <v>406</v>
       </c>
       <c r="H166" s="132" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I166" s="7"/>
       <c r="J166" s="7"/>
@@ -14109,7 +14106,7 @@
     </row>
     <row r="167">
       <c r="A167" s="63" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B167" s="73" t="s">
         <v>409</v>
@@ -14119,14 +14116,14 @@
       </c>
       <c r="D167" s="130"/>
       <c r="E167" s="131" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F167" s="131"/>
       <c r="G167" s="132" t="s">
         <v>412</v>
       </c>
       <c r="H167" s="132" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
@@ -14134,24 +14131,24 @@
     </row>
     <row r="168">
       <c r="A168" s="63" t="s">
+        <v>669</v>
+      </c>
+      <c r="B168" s="73" t="s">
         <v>670</v>
       </c>
-      <c r="B168" s="73" t="s">
-        <v>671</v>
-      </c>
       <c r="C168" s="129" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D168" s="130"/>
       <c r="E168" s="131" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F168" s="131"/>
       <c r="G168" s="132" t="s">
         <v>406</v>
       </c>
       <c r="H168" s="132" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I168" s="7"/>
       <c r="J168" s="7"/>
@@ -14159,7 +14156,7 @@
     </row>
     <row r="169">
       <c r="A169" s="63" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B169" s="73" t="s">
         <v>409</v>
@@ -14169,14 +14166,14 @@
       </c>
       <c r="D169" s="130"/>
       <c r="E169" s="131" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F169" s="131"/>
       <c r="G169" s="132" t="s">
         <v>412</v>
       </c>
       <c r="H169" s="132" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
@@ -14279,22 +14276,22 @@
     </row>
     <row r="2">
       <c r="A2" s="19" t="s">
+        <v>676</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>677</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="C2" s="74" t="s">
         <v>678</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="D2" s="74" t="s">
         <v>679</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="E2" s="39" t="s">
         <v>680</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="39" t="s">
         <v>681</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="3">
@@ -14309,15 +14306,15 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="39" t="s">
+        <v>682</v>
+      </c>
+      <c r="F3" s="39" t="s">
         <v>683</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="135" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B4" s="132" t="s">
         <v>349</v>
@@ -14325,10 +14322,10 @@
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
       <c r="E4" s="40" t="s">
+        <v>685</v>
+      </c>
+      <c r="F4" s="136" t="s">
         <v>686</v>
-      </c>
-      <c r="F4" s="136" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="5">
@@ -14345,10 +14342,10 @@
         <v>392</v>
       </c>
       <c r="E5" s="39" t="s">
+        <v>687</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>688</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>689</v>
       </c>
       <c r="G5" s="137"/>
       <c r="H5" s="137"/>
@@ -14381,10 +14378,10 @@
       <c r="C6" s="72"/>
       <c r="D6" s="72"/>
       <c r="E6" s="40" t="s">
+        <v>689</v>
+      </c>
+      <c r="F6" s="40" t="s">
         <v>690</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>691</v>
       </c>
       <c r="G6" s="137"/>
       <c r="H6" s="137"/>
@@ -14409,50 +14406,50 @@
     </row>
     <row r="7">
       <c r="A7" s="72" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B7" s="132" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C7" s="72"/>
       <c r="D7" s="72"/>
       <c r="E7" s="132" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F7" s="132" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="72" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B8" s="132" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C8" s="72"/>
       <c r="D8" s="72"/>
       <c r="E8" s="132" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F8" s="132" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="135" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B9" s="132" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C9" s="72"/>
       <c r="D9" s="72"/>
       <c r="E9" s="131" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F9" s="132" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10">
@@ -18445,36 +18442,36 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="138" t="s">
+        <v>695</v>
+      </c>
+      <c r="B2" s="139" t="s">
         <v>696</v>
-      </c>
-      <c r="B2" s="139" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="140" t="s">
+        <v>697</v>
+      </c>
+      <c r="B3" s="139" t="s">
         <v>698</v>
-      </c>
-      <c r="B3" s="139" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="141" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="142" t="s">
+        <v>700</v>
+      </c>
+      <c r="B6" s="139" t="s">
         <v>701</v>
-      </c>
-      <c r="B6" s="139" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="139" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="8">
@@ -18485,41 +18482,41 @@
     </row>
     <row r="10">
       <c r="A10" s="142" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="142" t="s">
+        <v>704</v>
+      </c>
+      <c r="B11" s="143" t="s">
         <v>705</v>
-      </c>
-      <c r="B11" s="143" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="144" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="145"/>
       <c r="B13" s="146" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="147" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="148" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="149" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="17">
@@ -18528,24 +18525,24 @@
     </row>
     <row r="18">
       <c r="A18" s="142" t="s">
+        <v>711</v>
+      </c>
+      <c r="B18" s="150" t="s">
         <v>712</v>
-      </c>
-      <c r="B18" s="150" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B19" s="151"/>
     </row>
     <row r="21">
       <c r="A21" s="142" t="s">
+        <v>714</v>
+      </c>
+      <c r="B21" s="152" t="s">
         <v>715</v>
-      </c>
-      <c r="B21" s="152" t="s">
-        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -18571,52 +18568,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="153" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="153" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="11">
@@ -18645,65 +18642,65 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B1" s="154" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>728</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="139" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="139" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="155" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B10" s="7"/>
     </row>
@@ -18748,10 +18745,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="156" t="s">
+        <v>737</v>
+      </c>
+      <c r="C1" s="156" t="s">
         <v>738</v>
-      </c>
-      <c r="C1" s="156" t="s">
-        <v>739</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -18778,16 +18775,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>742</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>743</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -18814,13 +18811,13 @@
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
+        <v>743</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>744</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="4" t="s">
         <v>745</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>746</v>
       </c>
       <c r="D3" s="4" t="str">
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
@@ -18851,13 +18848,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B4" s="39" t="s">
+        <v>744</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>745</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>746</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -18888,13 +18885,13 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
+        <v>747</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>748</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>749</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -18922,16 +18919,16 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>751</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>746</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>752</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -18958,16 +18955,16 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="D7" s="157" t="s">
         <v>754</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>746</v>
-      </c>
-      <c r="D7" s="157" t="s">
-        <v>755</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -18994,16 +18991,16 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>757</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>746</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>758</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -19030,16 +19027,16 @@
     </row>
     <row r="9">
       <c r="A9" s="158" t="s">
+        <v>758</v>
+      </c>
+      <c r="B9" s="159" t="s">
         <v>759</v>
       </c>
-      <c r="B9" s="159" t="s">
+      <c r="C9" s="159" t="s">
+        <v>745</v>
+      </c>
+      <c r="D9" s="159" t="s">
         <v>760</v>
-      </c>
-      <c r="C9" s="159" t="s">
-        <v>746</v>
-      </c>
-      <c r="D9" s="159" t="s">
-        <v>761</v>
       </c>
       <c r="E9" s="159"/>
       <c r="F9" s="159"/>
@@ -19066,16 +19063,16 @@
     </row>
     <row r="10">
       <c r="A10" s="158" t="s">
+        <v>761</v>
+      </c>
+      <c r="B10" s="159" t="s">
+        <v>759</v>
+      </c>
+      <c r="C10" s="159" t="s">
+        <v>745</v>
+      </c>
+      <c r="D10" s="159" t="s">
         <v>762</v>
-      </c>
-      <c r="B10" s="159" t="s">
-        <v>760</v>
-      </c>
-      <c r="C10" s="159" t="s">
-        <v>746</v>
-      </c>
-      <c r="D10" s="159" t="s">
-        <v>763</v>
       </c>
       <c r="E10" s="159"/>
       <c r="F10" s="159"/>
@@ -19102,16 +19099,16 @@
     </row>
     <row r="11">
       <c r="A11" s="158" t="s">
+        <v>763</v>
+      </c>
+      <c r="B11" s="159" t="s">
         <v>764</v>
       </c>
-      <c r="B11" s="159" t="s">
+      <c r="C11" s="159" t="s">
+        <v>745</v>
+      </c>
+      <c r="D11" s="159" t="s">
         <v>765</v>
-      </c>
-      <c r="C11" s="159" t="s">
-        <v>746</v>
-      </c>
-      <c r="D11" s="159" t="s">
-        <v>766</v>
       </c>
       <c r="E11" s="159"/>
       <c r="F11" s="159"/>
@@ -19138,16 +19135,16 @@
     </row>
     <row r="12">
       <c r="A12" s="158" t="s">
+        <v>766</v>
+      </c>
+      <c r="B12" s="159" t="s">
+        <v>764</v>
+      </c>
+      <c r="C12" s="159" t="s">
+        <v>745</v>
+      </c>
+      <c r="D12" s="159" t="s">
         <v>767</v>
-      </c>
-      <c r="B12" s="159" t="s">
-        <v>765</v>
-      </c>
-      <c r="C12" s="159" t="s">
-        <v>746</v>
-      </c>
-      <c r="D12" s="159" t="s">
-        <v>768</v>
       </c>
       <c r="E12" s="159"/>
       <c r="F12" s="159"/>
@@ -19174,16 +19171,16 @@
     </row>
     <row r="13">
       <c r="A13" s="158" t="s">
+        <v>768</v>
+      </c>
+      <c r="B13" s="158" t="s">
+        <v>748</v>
+      </c>
+      <c r="C13" s="159" t="s">
+        <v>745</v>
+      </c>
+      <c r="D13" s="159" t="s">
         <v>769</v>
-      </c>
-      <c r="B13" s="158" t="s">
-        <v>749</v>
-      </c>
-      <c r="C13" s="159" t="s">
-        <v>746</v>
-      </c>
-      <c r="D13" s="159" t="s">
-        <v>770</v>
       </c>
       <c r="E13" s="159"/>
       <c r="F13" s="159"/>
@@ -19210,16 +19207,16 @@
     </row>
     <row r="14">
       <c r="A14" s="158" t="s">
+        <v>770</v>
+      </c>
+      <c r="B14" s="158" t="s">
+        <v>748</v>
+      </c>
+      <c r="C14" s="159" t="s">
+        <v>745</v>
+      </c>
+      <c r="D14" s="159" t="s">
         <v>771</v>
-      </c>
-      <c r="B14" s="158" t="s">
-        <v>749</v>
-      </c>
-      <c r="C14" s="159" t="s">
-        <v>746</v>
-      </c>
-      <c r="D14" s="159" t="s">
-        <v>772</v>
       </c>
       <c r="E14" s="159"/>
       <c r="F14" s="159"/>
@@ -19271,51 +19268,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="160" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="142" t="s">
+        <v>739</v>
+      </c>
+      <c r="B2" s="142" t="s">
         <v>740</v>
       </c>
-      <c r="B2" s="142" t="s">
+      <c r="C2" s="142" t="s">
         <v>741</v>
       </c>
-      <c r="C2" s="142" t="s">
+      <c r="D2" s="142" t="s">
         <v>742</v>
-      </c>
-      <c r="D2" s="142" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="139" t="s">
+        <v>772</v>
+      </c>
+      <c r="B3" s="139" t="s">
         <v>773</v>
-      </c>
-      <c r="B3" s="139" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="139" t="s">
+        <v>774</v>
+      </c>
+      <c r="B4" s="139" t="s">
         <v>775</v>
-      </c>
-      <c r="B4" s="139" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="139" t="s">
+        <v>776</v>
+      </c>
+      <c r="B5" s="139" t="s">
         <v>777</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="C5" s="161" t="s">
+        <v>775</v>
+      </c>
+      <c r="D5" s="139" t="s">
         <v>778</v>
-      </c>
-      <c r="C5" s="161" t="s">
-        <v>776</v>
-      </c>
-      <c r="D5" s="139" t="s">
-        <v>779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CM for F20 in attempt to be make the CM diff tool run.
</commit_message>
<xml_diff>
--- a/mappings/package_F20/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F20/transformation/conceptual_mappings.xlsx
@@ -5027,6 +5027,12 @@
     </font>
     <font/>
     <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -5121,12 +5127,6 @@
     </font>
     <font>
       <color rgb="FFB7B7B7"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -5265,7 +5265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border/>
     <border>
       <left style="thin">
@@ -5312,6 +5312,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -5326,20 +5329,6 @@
     </border>
     <border>
       <bottom style="dotted">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -5429,8 +5418,8 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -5447,7 +5436,7 @@
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5492,7 +5481,7 @@
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="9" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -5568,22 +5557,22 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="9" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -5595,10 +5584,10 @@
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5622,10 +5611,10 @@
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5640,7 +5629,7 @@
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -5655,25 +5644,25 @@
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="4" fontId="23" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5682,60 +5671,60 @@
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -5747,20 +5736,20 @@
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">

</xml_diff>